<commit_message>
Added the interpolating function into the GBM pricers code
</commit_message>
<xml_diff>
--- a/excel_file/atm-volatility-surface.xlsx
+++ b/excel_file/atm-volatility-surface.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myresources.deloitte.com/personal/nerasmus_deloitte_co_za/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\excel_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A9FFE961-ED78-462D-9692-1F4049A272DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB877542-F3B3-4E05-8F2B-3FE0F3CFDA87}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6501FA-79C5-449B-A0C9-77D29C5545B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7360" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="vol-sruface" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,9 +46,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,17 +182,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +508,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,110 +529,110 @@
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>12.775</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>13.574999999999999</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>14.275</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <f>3/12</f>
         <v>0.25</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>14.55</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <f>6/12</f>
         <v>0.5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>14.9</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <f>9/12</f>
         <v>0.75</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>15.1</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+      <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>15.4</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+      <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>15.45</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+      <c r="A10" s="4">
         <v>3</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>15.885</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
         <v>15.945</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+      <c r="A12" s="4">
         <v>7</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>15.12</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>15</v>
       </c>
       <c r="C13" s="1"/>

</xml_diff>